<commit_message>
change test data on new site
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/v5DataProvider.xlsx
+++ b/src/test/resources/fixtures/v5DataProvider.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="152">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -628,18 +628,10 @@
     <t>brian</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="14"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>brian@example.com</t>
-    </r>
+    <t>brian1@example.com</t>
   </si>
   <si>
-    <t>123456789</t>
+    <t>123456</t>
   </si>
   <si>
     <t>/brian</t>
@@ -651,15 +643,7 @@
     <t>terry</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="14"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>terry@example.net</t>
-    </r>
+    <t>terry1@example.net</t>
   </si>
   <si>
     <t>/terry</t>
@@ -675,10 +659,10 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="14"/>
+        <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>luna@example.net</t>
+      <t>luna1@example.net</t>
     </r>
   </si>
   <si>
@@ -691,7 +675,7 @@
     <t>katie</t>
   </si>
   <si>
-    <t>katie@example.net</t>
+    <t>katie1@example.net</t>
   </si>
   <si>
     <t>/katie</t>
@@ -700,13 +684,38 @@
     <t>test</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>terry@example.net</t>
+    </r>
+  </si>
+  <si>
     <t>/test</t>
   </si>
   <si>
     <t>file</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>brian@example.com</t>
+    </r>
+  </si>
+  <si>
     <t>luna@example.net</t>
+  </si>
+  <si>
+    <t>katie@example.net</t>
   </si>
 </sst>
 </file>
@@ -716,7 +725,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -770,6 +779,12 @@
       <color indexed="15"/>
       <name val="Consolas"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -792,7 +807,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -807,11 +822,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -820,7 +835,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -828,17 +843,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
@@ -855,7 +870,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -863,12 +878,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -877,18 +903,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -912,43 +927,43 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -980,28 +995,28 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1019,20 +1034,20 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -1123,8 +1138,8 @@
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff1155cc"/>
       <rgbColor rgb="ff202124"/>
     </indexedColors>
@@ -2211,7 +2226,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2389,16 +2404,19 @@
       <c r="D18" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="E18" s="24"/>
-    </row>
-    <row r="19">
+      <c r="E18" s="21"/>
+    </row>
+    <row r="19" ht="13" customHeight="1">
+      <c r="A19" s="7"/>
       <c r="B19" t="s" s="3">
         <v>14</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-    </row>
-    <row r="20">
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" ht="13" customHeight="1">
+      <c r="A20" s="20"/>
       <c r="B20" s="4"/>
       <c r="C20" t="s" s="4">
         <v>5</v>
@@ -2406,6 +2424,7 @@
       <c r="D20" t="s" s="5">
         <v>14</v>
       </c>
+      <c r="E20" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2415,10 +2434,11 @@
   <hyperlinks>
     <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'browserConfig'!R1C1" tooltip="" display="browserConfig"/>
-    <hyperlink ref="D12" location="'blogs'!R1C1" tooltip="" display="blogs"/>
-    <hyperlink ref="D14" location="'pages'!R1C1" tooltip="" display="pages"/>
-    <hyperlink ref="D16" location="'users'!R1C1" tooltip="" display="users"/>
-    <hyperlink ref="D18" location="'photos'!R1C1" tooltip="" display="photos"/>
+    <hyperlink ref="D12" location="'browserConfig'!R1C1" tooltip="" display="browserConfig"/>
+    <hyperlink ref="D14" location="'blogs'!R1C1" tooltip="" display="blogs"/>
+    <hyperlink ref="D16" location="'pages'!R1C1" tooltip="" display="pages"/>
+    <hyperlink ref="D18" location="'users'!R1C1" tooltip="" display="users"/>
+    <hyperlink ref="D20" location="'photos'!R1C1" tooltip="" display="photos"/>
     <hyperlink ref="D12" location="'browserConfig'!R1C1" tooltip="" display="browserConfig"/>
     <hyperlink ref="D14" location="'blogs'!R1C1" tooltip="" display="blogs"/>
     <hyperlink ref="D16" location="'pages'!R1C1" tooltip="" display="pages"/>
@@ -6544,13 +6564,13 @@
         <v>145</v>
       </c>
       <c r="E7" t="s" s="39">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="F7" t="s" s="44">
         <v>131</v>
       </c>
       <c r="G7" t="s" s="39">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H7" t="s" s="41">
         <v>127</v>
@@ -36398,18 +36418,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" location="" tooltip="" display="brian@example.com"/>
-    <hyperlink ref="E4" r:id="rId2" location="" tooltip="" display="terry@example.net"/>
-    <hyperlink ref="E5" r:id="rId3" location="" tooltip="" display="luna@example.net"/>
-    <hyperlink ref="E7" r:id="rId4" location="" tooltip="" display="terry@example.net"/>
+    <hyperlink ref="E5" r:id="rId1" location="" tooltip="" display="luna1@example.net"/>
+    <hyperlink ref="E7" r:id="rId2" location="" tooltip="" display="terry@example.net"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -36438,7 +36456,7 @@
         <v>17</v>
       </c>
       <c r="C1" t="s" s="35">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s" s="35">
         <v>119</v>
@@ -36522,7 +36540,7 @@
         <v>129</v>
       </c>
       <c r="E3" t="s" s="39">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="F3" s="47">
         <v>123456</v>
@@ -36559,7 +36577,7 @@
         <v>134</v>
       </c>
       <c r="E4" t="s" s="39">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="F4" s="47">
         <v>123456</v>
@@ -36596,7 +36614,7 @@
         <v>138</v>
       </c>
       <c r="E5" t="s" s="39">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F5" s="47">
         <v>123456</v>
@@ -36633,7 +36651,7 @@
         <v>142</v>
       </c>
       <c r="E6" t="s" s="39">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="F6" s="47">
         <v>123456</v>

</xml_diff>

<commit_message>
change test case on new site
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/v5DataProvider.xlsx
+++ b/src/test/resources/fixtures/v5DataProvider.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="153">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -652,7 +652,7 @@
     <t>Luna</t>
   </si>
   <si>
-    <t>luna</t>
+    <t>krixi</t>
   </si>
   <si>
     <r>
@@ -710,6 +710,9 @@
       </rPr>
       <t>brian@example.com</t>
     </r>
+  </si>
+  <si>
+    <t>luna</t>
   </si>
   <si>
     <t>luna@example.net</t>
@@ -36611,10 +36614,10 @@
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
       <c r="D5" t="s" s="39">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="E5" t="s" s="39">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F5" s="47">
         <v>123456</v>
@@ -36651,7 +36654,7 @@
         <v>142</v>
       </c>
       <c r="E6" t="s" s="39">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F6" s="47">
         <v>123456</v>

</xml_diff>

<commit_message>
add test case on Saved items
</commit_message>
<xml_diff>
--- a/src/test/resources/fixtures/v5DataProvider.xlsx
+++ b/src/test/resources/fixtures/v5DataProvider.xlsx
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="159">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -613,7 +613,15 @@
     <t>admin</t>
   </si>
   <si>
-    <t>dev@phpfox.com</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>dev@phpfox.com</t>
+    </r>
   </si>
   <si>
     <t>bubble666</t>
@@ -694,6 +702,9 @@
   </si>
   <si>
     <t>file</t>
+  </si>
+  <si>
+    <t>dev@phpfox.com</t>
   </si>
   <si>
     <t>brian</t>
@@ -36436,15 +36447,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" location="" tooltip="" display="luna1@example.net"/>
+    <hyperlink ref="E2" r:id="rId1" location="" tooltip="" display="dev@phpfox.com"/>
+    <hyperlink ref="E5" r:id="rId2" location="" tooltip="" display="luna1@example.net"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -36520,7 +36532,7 @@
         <v>124</v>
       </c>
       <c r="E2" t="s" s="39">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="F2" t="s" s="44">
         <v>126</v>
@@ -36554,10 +36566,10 @@
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
       <c r="D3" t="s" s="39">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E3" t="s" s="39">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F3" s="47">
         <v>123456</v>
@@ -36591,10 +36603,10 @@
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
       <c r="D4" t="s" s="39">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E4" t="s" s="39">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F4" s="47">
         <v>123456</v>
@@ -36628,10 +36640,10 @@
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
       <c r="D5" t="s" s="39">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E5" t="s" s="39">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F5" s="47">
         <v>123456</v>
@@ -36665,10 +36677,10 @@
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
       <c r="D6" t="s" s="39">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E6" t="s" s="39">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F6" s="47">
         <v>123456</v>

</xml_diff>